<commit_message>
Updating Miro Data scenarios
</commit_message>
<xml_diff>
--- a/src/test/java/com/miro/data/miro_data.xlsx
+++ b/src/test/java/com/miro/data/miro_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcardena\Desktop\Matías\Automation\Java\miro-test-automation\src\test\java\com\miro\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B867A6B2-006B-48C0-AF7E-473391885E8A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78C3E8B4-51C2-446D-9F77-95808F122F20}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{30F17799-0A18-4BA2-A76D-8633784C3C58}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="10">
   <si>
     <t>email</t>
   </si>
@@ -171,7 +171,1140 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="19">
+  <dxfs count="174">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -627,10 +1760,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{747DD830-0D78-4AB6-92E0-8F370C84190E}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+      <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -709,76 +1842,748 @@
         <v>9</v>
       </c>
     </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="C5 C2:C3">
-    <cfRule type="expression" dxfId="18" priority="104">
-      <formula>"MISSING"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="17" priority="105">
-      <formula>"EMPTY"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="16" priority="106">
-      <formula>"""FILLED"""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A2:D5">
-    <cfRule type="containsText" dxfId="15" priority="101" operator="containsText" text="EMPTY">
+    <cfRule type="expression" dxfId="173" priority="265">
+      <formula>"MISSING"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="172" priority="266">
+      <formula>"EMPTY"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="171" priority="267">
+      <formula>"""FILLED"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B9:D9 A7:A8 A2:D7 C8:D8">
+    <cfRule type="containsText" dxfId="170" priority="262" operator="containsText" text="EMPTY">
       <formula>NOT(ISERROR(SEARCH("EMPTY",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="102" operator="containsText" text="MISSING">
+    <cfRule type="containsText" dxfId="169" priority="263" operator="containsText" text="MISSING">
       <formula>NOT(ISERROR(SEARCH("MISSING",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="103" operator="containsText" text="FILLED">
+    <cfRule type="containsText" dxfId="168" priority="264" operator="containsText" text="FILLED">
       <formula>NOT(ISERROR(SEARCH("FILLED",A2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2">
-    <cfRule type="expression" dxfId="12" priority="14">
-      <formula>"MISSING"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="11" priority="15">
-      <formula>"EMPTY"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="10" priority="16">
+    <cfRule type="expression" dxfId="167" priority="175">
+      <formula>"MISSING"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="166" priority="176">
+      <formula>"EMPTY"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="165" priority="177">
       <formula>"""FILLED"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4">
-    <cfRule type="expression" dxfId="9" priority="11">
-      <formula>"MISSING"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="8" priority="12">
-      <formula>"EMPTY"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="7" priority="13">
+    <cfRule type="expression" dxfId="164" priority="172">
+      <formula>"MISSING"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="163" priority="173">
+      <formula>"EMPTY"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="162" priority="174">
       <formula>"""FILLED"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4">
-    <cfRule type="expression" dxfId="6" priority="5">
-      <formula>"MISSING"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="5" priority="6">
-      <formula>"EMPTY"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="4" priority="7">
+    <cfRule type="expression" dxfId="161" priority="166">
+      <formula>"MISSING"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="160" priority="167">
+      <formula>"EMPTY"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="159" priority="168">
       <formula>"""FILLED"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4">
-    <cfRule type="expression" dxfId="3" priority="2">
-      <formula>"MISSING"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="2" priority="3">
-      <formula>"EMPTY"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="4">
+    <cfRule type="expression" dxfId="158" priority="163">
+      <formula>"MISSING"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="157" priority="164">
+      <formula>"EMPTY"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="156" priority="165">
       <formula>"""FILLED"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="155" priority="162">
       <formula>"SELECTED"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C9 C6:C7">
+    <cfRule type="expression" dxfId="154" priority="159">
+      <formula>"MISSING"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="153" priority="160">
+      <formula>"EMPTY"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="152" priority="161">
+      <formula>"""FILLED"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C8">
+    <cfRule type="expression" dxfId="151" priority="150">
+      <formula>"MISSING"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="150" priority="151">
+      <formula>"EMPTY"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="149" priority="152">
+      <formula>"""FILLED"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A8">
+    <cfRule type="expression" dxfId="148" priority="147">
+      <formula>"MISSING"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="147" priority="148">
+      <formula>"EMPTY"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="146" priority="149">
+      <formula>"""FILLED"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C8">
+    <cfRule type="expression" dxfId="145" priority="144">
+      <formula>"MISSING"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="144" priority="145">
+      <formula>"EMPTY"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="143" priority="146">
+      <formula>"""FILLED"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D6">
+    <cfRule type="expression" dxfId="142" priority="143">
+      <formula>"SELECTED"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C13 C10:C11">
+    <cfRule type="expression" dxfId="141" priority="140">
+      <formula>"MISSING"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="140" priority="141">
+      <formula>"EMPTY"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="139" priority="142">
+      <formula>"""FILLED"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A10:D13">
+    <cfRule type="containsText" dxfId="138" priority="137" operator="containsText" text="EMPTY">
+      <formula>NOT(ISERROR(SEARCH("EMPTY",A10)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="137" priority="138" operator="containsText" text="MISSING">
+      <formula>NOT(ISERROR(SEARCH("MISSING",A10)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="136" priority="139" operator="containsText" text="FILLED">
+      <formula>NOT(ISERROR(SEARCH("FILLED",A10)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A10">
+    <cfRule type="expression" dxfId="135" priority="134">
+      <formula>"MISSING"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="134" priority="135">
+      <formula>"EMPTY"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="133" priority="136">
+      <formula>"""FILLED"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C12">
+    <cfRule type="expression" dxfId="132" priority="131">
+      <formula>"MISSING"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="131" priority="132">
+      <formula>"EMPTY"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="130" priority="133">
+      <formula>"""FILLED"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A12">
+    <cfRule type="expression" dxfId="129" priority="128">
+      <formula>"MISSING"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="128" priority="129">
+      <formula>"EMPTY"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="127" priority="130">
+      <formula>"""FILLED"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C12">
+    <cfRule type="expression" dxfId="126" priority="125">
+      <formula>"MISSING"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="125" priority="126">
+      <formula>"EMPTY"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="124" priority="127">
+      <formula>"""FILLED"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D10">
+    <cfRule type="expression" dxfId="123" priority="124">
+      <formula>"SELECTED"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A7">
+    <cfRule type="expression" dxfId="122" priority="121">
+      <formula>"MISSING"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="121" priority="122">
+      <formula>"EMPTY"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="120" priority="123">
+      <formula>"""FILLED"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B7">
+    <cfRule type="expression" dxfId="119" priority="118">
+      <formula>"MISSING"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="118" priority="119">
+      <formula>"EMPTY"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="117" priority="120">
+      <formula>"""FILLED"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A7">
+    <cfRule type="expression" dxfId="116" priority="115">
+      <formula>"MISSING"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="115" priority="116">
+      <formula>"EMPTY"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="114" priority="117">
+      <formula>"""FILLED"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A7">
+    <cfRule type="expression" dxfId="113" priority="112">
+      <formula>"MISSING"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="112" priority="113">
+      <formula>"EMPTY"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="111" priority="114">
+      <formula>"""FILLED"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C7">
+    <cfRule type="expression" dxfId="110" priority="109">
+      <formula>"MISSING"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="109" priority="110">
+      <formula>"EMPTY"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="108" priority="111">
+      <formula>"""FILLED"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C7">
+    <cfRule type="expression" dxfId="107" priority="106">
+      <formula>"MISSING"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="106" priority="107">
+      <formula>"EMPTY"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="105" priority="108">
+      <formula>"""FILLED"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A7">
+    <cfRule type="expression" dxfId="104" priority="103">
+      <formula>"MISSING"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="103" priority="104">
+      <formula>"EMPTY"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="102" priority="105">
+      <formula>"""FILLED"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C8">
+    <cfRule type="expression" dxfId="101" priority="100">
+      <formula>"MISSING"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="100" priority="101">
+      <formula>"EMPTY"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="99" priority="102">
+      <formula>"""FILLED"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C8">
+    <cfRule type="expression" dxfId="98" priority="97">
+      <formula>"MISSING"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="97" priority="98">
+      <formula>"EMPTY"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="96" priority="99">
+      <formula>"""FILLED"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C8">
+    <cfRule type="expression" dxfId="95" priority="94">
+      <formula>"MISSING"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="94" priority="95">
+      <formula>"EMPTY"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="93" priority="96">
+      <formula>"""FILLED"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C6">
+    <cfRule type="expression" dxfId="92" priority="91">
+      <formula>"MISSING"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="91" priority="92">
+      <formula>"EMPTY"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="90" priority="93">
+      <formula>"""FILLED"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C6">
+    <cfRule type="expression" dxfId="89" priority="88">
+      <formula>"MISSING"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="88" priority="89">
+      <formula>"EMPTY"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="87" priority="90">
+      <formula>"""FILLED"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C6">
+    <cfRule type="expression" dxfId="86" priority="85">
+      <formula>"MISSING"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="85" priority="86">
+      <formula>"EMPTY"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="84" priority="87">
+      <formula>"""FILLED"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C6">
+    <cfRule type="expression" dxfId="83" priority="82">
+      <formula>"MISSING"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="82" priority="83">
+      <formula>"EMPTY"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="81" priority="84">
+      <formula>"""FILLED"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C6">
+    <cfRule type="expression" dxfId="80" priority="79">
+      <formula>"MISSING"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="79" priority="80">
+      <formula>"EMPTY"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="78" priority="81">
+      <formula>"""FILLED"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A7">
+    <cfRule type="expression" dxfId="77" priority="76">
+      <formula>"MISSING"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="76" priority="77">
+      <formula>"EMPTY"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="75" priority="78">
+      <formula>"""FILLED"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C7">
+    <cfRule type="expression" dxfId="74" priority="73">
+      <formula>"MISSING"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="73" priority="74">
+      <formula>"EMPTY"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="72" priority="75">
+      <formula>"""FILLED"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C7">
+    <cfRule type="expression" dxfId="71" priority="70">
+      <formula>"MISSING"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="70" priority="71">
+      <formula>"EMPTY"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="69" priority="72">
+      <formula>"""FILLED"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C7">
+    <cfRule type="expression" dxfId="68" priority="67">
+      <formula>"MISSING"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="67" priority="68">
+      <formula>"EMPTY"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="66" priority="69">
+      <formula>"""FILLED"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C7">
+    <cfRule type="expression" dxfId="65" priority="64">
+      <formula>"MISSING"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="64" priority="65">
+      <formula>"EMPTY"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="63" priority="66">
+      <formula>"""FILLED"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C7">
+    <cfRule type="expression" dxfId="62" priority="61">
+      <formula>"MISSING"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="61" priority="62">
+      <formula>"EMPTY"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="60" priority="63">
+      <formula>"""FILLED"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B6">
+    <cfRule type="expression" dxfId="56" priority="55">
+      <formula>"MISSING"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="55" priority="56">
+      <formula>"EMPTY"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="54" priority="57">
+      <formula>"""FILLED"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B6">
+    <cfRule type="expression" dxfId="53" priority="52">
+      <formula>"MISSING"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="52" priority="53">
+      <formula>"EMPTY"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="51" priority="54">
+      <formula>"""FILLED"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C6">
+    <cfRule type="expression" dxfId="50" priority="49">
+      <formula>"MISSING"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="49" priority="50">
+      <formula>"EMPTY"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="48" priority="51">
+      <formula>"""FILLED"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C6">
+    <cfRule type="expression" dxfId="47" priority="46">
+      <formula>"MISSING"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="46" priority="47">
+      <formula>"EMPTY"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="45" priority="48">
+      <formula>"""FILLED"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B7">
+    <cfRule type="expression" dxfId="44" priority="43">
+      <formula>"MISSING"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="43" priority="44">
+      <formula>"EMPTY"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="42" priority="45">
+      <formula>"""FILLED"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B7">
+    <cfRule type="expression" dxfId="41" priority="40">
+      <formula>"MISSING"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="40" priority="41">
+      <formula>"EMPTY"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="39" priority="42">
+      <formula>"""FILLED"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B8">
+    <cfRule type="containsText" dxfId="38" priority="37" operator="containsText" text="EMPTY">
+      <formula>NOT(ISERROR(SEARCH("EMPTY",B8)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="37" priority="38" operator="containsText" text="MISSING">
+      <formula>NOT(ISERROR(SEARCH("MISSING",B8)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="36" priority="39" operator="containsText" text="FILLED">
+      <formula>NOT(ISERROR(SEARCH("FILLED",B8)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B8">
+    <cfRule type="expression" dxfId="35" priority="34">
+      <formula>"MISSING"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="34" priority="35">
+      <formula>"EMPTY"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="33" priority="36">
+      <formula>"""FILLED"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B8">
+    <cfRule type="expression" dxfId="32" priority="31">
+      <formula>"MISSING"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="31" priority="32">
+      <formula>"EMPTY"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="30" priority="33">
+      <formula>"""FILLED"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C8">
+    <cfRule type="expression" dxfId="29" priority="28">
+      <formula>"MISSING"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="28" priority="29">
+      <formula>"EMPTY"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="27" priority="30">
+      <formula>"""FILLED"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C8">
+    <cfRule type="expression" dxfId="26" priority="25">
+      <formula>"MISSING"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="25" priority="26">
+      <formula>"EMPTY"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="24" priority="27">
+      <formula>"""FILLED"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A9">
+    <cfRule type="containsText" dxfId="23" priority="22" operator="containsText" text="EMPTY">
+      <formula>NOT(ISERROR(SEARCH("EMPTY",A9)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="22" priority="23" operator="containsText" text="MISSING">
+      <formula>NOT(ISERROR(SEARCH("MISSING",A9)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="21" priority="24" operator="containsText" text="FILLED">
+      <formula>NOT(ISERROR(SEARCH("FILLED",A9)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A9">
+    <cfRule type="expression" dxfId="20" priority="19">
+      <formula>"MISSING"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="19" priority="20">
+      <formula>"EMPTY"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="18" priority="21">
+      <formula>"""FILLED"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A9">
+    <cfRule type="expression" dxfId="17" priority="16">
+      <formula>"MISSING"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="16" priority="17">
+      <formula>"EMPTY"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="15" priority="18">
+      <formula>"""FILLED"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A11">
+    <cfRule type="expression" dxfId="14" priority="13">
+      <formula>"MISSING"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="13" priority="14">
+      <formula>"EMPTY"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="12" priority="15">
+      <formula>"""FILLED"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A12">
+    <cfRule type="expression" dxfId="11" priority="10">
+      <formula>"MISSING"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="10" priority="11">
+      <formula>"EMPTY"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="9" priority="12">
+      <formula>"""FILLED"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C12">
+    <cfRule type="expression" dxfId="8" priority="7">
+      <formula>"MISSING"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="7" priority="8">
+      <formula>"EMPTY"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="9">
+      <formula>"""FILLED"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A13">
+    <cfRule type="expression" dxfId="5" priority="4">
+      <formula>"MISSING"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="5">
+      <formula>"EMPTY"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="3" priority="6">
+      <formula>"""FILLED"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A13">
+    <cfRule type="expression" dxfId="2" priority="1">
+      <formula>"MISSING"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>"EMPTY"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="3">
+      <formula>"""FILLED"""</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -786,17 +2591,17 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{39245428-C064-4004-97CD-08D187C3CA6E}">
+          <x14:formula1>
+            <xm:f>Lists!$C$2:$C$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>D2:D13</xm:sqref>
+        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F9E7F89B-8139-43AF-8396-985A9BD83313}">
           <x14:formula1>
             <xm:f>Lists!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>A2:C5</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{39245428-C064-4004-97CD-08D187C3CA6E}">
-          <x14:formula1>
-            <xm:f>Lists!$C$2:$C$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>D2:D5</xm:sqref>
+          <xm:sqref>A2:C13</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>